<commit_message>
ADD RECUPERAÇÃO E MAPA FINAL
</commit_message>
<xml_diff>
--- a/statics/MAPAPARCIAL1_2023_INTEGRAL.xlsx
+++ b/statics/MAPAPARCIAL1_2023_INTEGRAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27204"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f28ae49758e922e1/Desktop/devbook/editabletable/statics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{2A5719C1-1E77-4370-92AE-51FA9A405023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07CF6838-4BAE-46C7-B7B3-C40957C360C0}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{2A5719C1-1E77-4370-92AE-51FA9A405023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92A3F5D8-C1D5-4D5C-9FB8-C9E9E8465CFC}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="11295" xr2:uid="{BCAD9878-E9D0-420E-8A55-493979D05A8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{BCAD9878-E9D0-420E-8A55-493979D05A8F}"/>
   </bookViews>
   <sheets>
     <sheet name="con" sheetId="1" r:id="rId1"/>
@@ -706,9 +706,9 @@
   </sheetPr>
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X4" sqref="X4"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>